<commit_message>
uppdaterat WBS med prelimenär tidsåtgång
</commit_message>
<xml_diff>
--- a/Bolaget/Temp/WBS v.1.xlsx
+++ b/Bolaget/Temp/WBS v.1.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beije\Documents\Projektkurs DVA227\Bolaget\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B16626E-88E4-4452-8742-D4F63FFD9ED5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5784"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="306">
   <si>
     <t>Nätverkstjänster</t>
   </si>
@@ -939,13 +940,16 @@
   </si>
   <si>
     <t>Vem ska göra vad på rapporten, vem skriver vilken del?</t>
+  </si>
+  <si>
+    <t>Prelimenär arbetsåtgång:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -983,8 +987,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1012,6 +1023,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1037,13 +1053,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -1053,10 +1070,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Beräkning" xfId="3" builtinId="22"/>
     <cellStyle name="Bra" xfId="1" builtinId="26"/>
+    <cellStyle name="Indata" xfId="4" builtinId="20"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1369,11 +1388,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I132"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="H121" sqref="H121"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="H134" sqref="H134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1413,7 +1432,9 @@
         <v>1</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5">
+        <v>4</v>
+      </c>
       <c r="I4" t="s">
         <v>101</v>
       </c>
@@ -1425,7 +1446,9 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="5">
+        <v>4</v>
+      </c>
       <c r="I5" t="s">
         <v>102</v>
       </c>
@@ -1437,7 +1460,9 @@
       <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
       <c r="I6" t="s">
         <v>103</v>
       </c>
@@ -1449,7 +1474,9 @@
       <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
       <c r="I7" t="s">
         <v>104</v>
       </c>
@@ -1461,7 +1488,9 @@
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
       <c r="I8" t="s">
         <v>105</v>
       </c>
@@ -1473,7 +1502,9 @@
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
       <c r="I9" t="s">
         <v>106</v>
       </c>
@@ -1485,7 +1516,9 @@
       <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
       <c r="I10" t="s">
         <v>107</v>
       </c>
@@ -1497,7 +1530,9 @@
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
       <c r="I11" t="s">
         <v>108</v>
       </c>
@@ -1509,7 +1544,9 @@
       <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
       <c r="I12" t="s">
         <v>109</v>
       </c>
@@ -1521,7 +1558,9 @@
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
       <c r="I13" t="s">
         <v>110</v>
       </c>
@@ -1533,7 +1572,9 @@
       <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="5">
+        <v>1</v>
+      </c>
       <c r="I14" t="s">
         <v>111</v>
       </c>
@@ -1554,7 +1595,9 @@
       <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="5">
+        <v>2</v>
+      </c>
       <c r="I16" t="s">
         <v>112</v>
       </c>
@@ -1566,7 +1609,9 @@
       <c r="D17" t="s">
         <v>14</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="5">
+        <v>1</v>
+      </c>
       <c r="I17" t="s">
         <v>113</v>
       </c>
@@ -1579,7 +1624,9 @@
         <v>15</v>
       </c>
       <c r="D18" s="2"/>
-      <c r="F18" s="5"/>
+      <c r="F18" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
@@ -1588,7 +1635,9 @@
       <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="5">
+        <v>2</v>
+      </c>
       <c r="I19" t="s">
         <v>114</v>
       </c>
@@ -1600,7 +1649,9 @@
       <c r="D20" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="5">
+        <v>2</v>
+      </c>
       <c r="I20" t="s">
         <v>115</v>
       </c>
@@ -1613,7 +1664,9 @@
         <v>18</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="F21" s="5"/>
+      <c r="F21" s="5">
+        <v>1</v>
+      </c>
       <c r="I21" t="s">
         <v>116</v>
       </c>
@@ -1625,7 +1678,9 @@
       <c r="D22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="5"/>
+      <c r="F22" s="5">
+        <v>1</v>
+      </c>
       <c r="I22" t="s">
         <v>117</v>
       </c>
@@ -1637,7 +1692,9 @@
       <c r="D23" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="5"/>
+      <c r="F23" s="5">
+        <v>1</v>
+      </c>
       <c r="I23" t="s">
         <v>118</v>
       </c>
@@ -1649,7 +1706,9 @@
       <c r="D24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="5">
+        <v>1</v>
+      </c>
       <c r="I24" t="s">
         <v>119</v>
       </c>
@@ -1662,7 +1721,9 @@
         <v>22</v>
       </c>
       <c r="D25" s="2"/>
-      <c r="F25" s="5"/>
+      <c r="F25" s="5">
+        <v>2</v>
+      </c>
       <c r="I25" t="s">
         <v>120</v>
       </c>
@@ -1674,7 +1735,9 @@
       <c r="D26" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="5"/>
+      <c r="F26" s="5">
+        <v>1</v>
+      </c>
       <c r="I26" t="s">
         <v>122</v>
       </c>
@@ -1686,7 +1749,9 @@
       <c r="D27" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="5"/>
+      <c r="F27" s="5">
+        <v>1</v>
+      </c>
       <c r="I27" t="s">
         <v>121</v>
       </c>
@@ -1698,7 +1763,9 @@
       <c r="D28" t="s">
         <v>17</v>
       </c>
-      <c r="F28" s="5"/>
+      <c r="F28" s="5">
+        <v>1</v>
+      </c>
       <c r="I28" t="s">
         <v>123</v>
       </c>
@@ -1710,7 +1777,9 @@
       <c r="C29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="5"/>
+      <c r="F29" s="5">
+        <v>4</v>
+      </c>
       <c r="I29" t="s">
         <v>124</v>
       </c>
@@ -1722,7 +1791,9 @@
       <c r="D30" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="5">
+        <v>2</v>
+      </c>
       <c r="I30" t="s">
         <v>125</v>
       </c>
@@ -1734,7 +1805,9 @@
       <c r="D31" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="5"/>
+      <c r="F31" s="5">
+        <v>2</v>
+      </c>
       <c r="I31" t="s">
         <v>126</v>
       </c>
@@ -1746,7 +1819,9 @@
       <c r="D32" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="5"/>
+      <c r="F32" s="5">
+        <v>2</v>
+      </c>
       <c r="I32" t="s">
         <v>127</v>
       </c>
@@ -1758,7 +1833,9 @@
       <c r="C33" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F33" s="5"/>
+      <c r="F33" s="5">
+        <v>2</v>
+      </c>
       <c r="I33" t="s">
         <v>128</v>
       </c>
@@ -1770,7 +1847,9 @@
       <c r="D34" t="s">
         <v>28</v>
       </c>
-      <c r="F34" s="5"/>
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
       <c r="I34" t="s">
         <v>129</v>
       </c>
@@ -1791,7 +1870,9 @@
       <c r="C36" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F36" s="5"/>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
       <c r="I36" t="s">
         <v>130</v>
       </c>
@@ -1803,7 +1884,9 @@
       <c r="D37" t="s">
         <v>31</v>
       </c>
-      <c r="F37" s="5"/>
+      <c r="F37" s="5">
+        <v>1</v>
+      </c>
       <c r="I37" t="s">
         <v>131</v>
       </c>
@@ -1815,7 +1898,9 @@
       <c r="D38" t="s">
         <v>32</v>
       </c>
-      <c r="F38" s="5"/>
+      <c r="F38" s="5">
+        <v>3</v>
+      </c>
       <c r="I38" t="s">
         <v>132</v>
       </c>
@@ -1827,7 +1912,9 @@
       <c r="C39" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F39" s="5"/>
+      <c r="F39" s="5">
+        <v>4</v>
+      </c>
       <c r="I39" t="s">
         <v>133</v>
       </c>
@@ -1839,7 +1926,9 @@
       <c r="D40" t="s">
         <v>34</v>
       </c>
-      <c r="F40" s="5"/>
+      <c r="F40" s="5">
+        <v>1</v>
+      </c>
       <c r="I40" t="s">
         <v>134</v>
       </c>
@@ -1851,7 +1940,9 @@
       <c r="D41" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="5"/>
+      <c r="F41" s="5">
+        <v>3</v>
+      </c>
       <c r="I41" t="s">
         <v>135</v>
       </c>
@@ -1863,7 +1954,9 @@
       <c r="C42" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F42" s="5"/>
+      <c r="F42" s="5">
+        <v>3</v>
+      </c>
       <c r="I42" t="s">
         <v>136</v>
       </c>
@@ -1875,7 +1968,9 @@
       <c r="D43" t="s">
         <v>37</v>
       </c>
-      <c r="F43" s="5"/>
+      <c r="F43" s="5">
+        <v>3</v>
+      </c>
       <c r="I43" t="s">
         <v>137</v>
       </c>
@@ -1887,7 +1982,9 @@
       <c r="D44" t="s">
         <v>38</v>
       </c>
-      <c r="F44" s="5"/>
+      <c r="F44" s="5">
+        <v>2</v>
+      </c>
       <c r="I44" t="s">
         <v>138</v>
       </c>
@@ -1900,7 +1997,9 @@
         <v>39</v>
       </c>
       <c r="D45" s="4"/>
-      <c r="F45" s="5"/>
+      <c r="F45" s="5">
+        <v>2</v>
+      </c>
       <c r="I45" t="s">
         <v>139</v>
       </c>
@@ -1912,7 +2011,9 @@
       <c r="D46" t="s">
         <v>40</v>
       </c>
-      <c r="F46" s="5"/>
+      <c r="F46" s="5">
+        <v>2</v>
+      </c>
       <c r="I46" t="s">
         <v>140</v>
       </c>
@@ -1934,7 +2035,9 @@
         <v>42</v>
       </c>
       <c r="D48" s="2"/>
-      <c r="F48" s="5"/>
+      <c r="F48" s="5">
+        <v>3</v>
+      </c>
       <c r="I48" t="s">
         <v>141</v>
       </c>
@@ -1946,7 +2049,9 @@
       <c r="D49" t="s">
         <v>43</v>
       </c>
-      <c r="F49" s="5"/>
+      <c r="F49" s="5">
+        <v>2</v>
+      </c>
       <c r="I49" t="s">
         <v>142</v>
       </c>
@@ -1958,7 +2063,9 @@
       <c r="D50" t="s">
         <v>44</v>
       </c>
-      <c r="F50" s="5"/>
+      <c r="F50" s="5">
+        <v>2</v>
+      </c>
       <c r="I50" t="s">
         <v>143</v>
       </c>
@@ -1970,7 +2077,9 @@
       <c r="D51" t="s">
         <v>45</v>
       </c>
-      <c r="F51" s="5"/>
+      <c r="F51" s="5">
+        <v>1</v>
+      </c>
       <c r="I51" t="s">
         <v>144</v>
       </c>
@@ -1982,7 +2091,9 @@
       <c r="D52" t="s">
         <v>12</v>
       </c>
-      <c r="F52" s="5"/>
+      <c r="F52" s="5">
+        <v>2</v>
+      </c>
       <c r="I52" t="s">
         <v>145</v>
       </c>
@@ -1994,7 +2105,9 @@
       <c r="C53" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F53" s="5"/>
+      <c r="F53" s="5">
+        <v>1</v>
+      </c>
       <c r="I53" t="s">
         <v>146</v>
       </c>
@@ -2006,7 +2119,9 @@
       <c r="D54" t="s">
         <v>47</v>
       </c>
-      <c r="F54" s="5"/>
+      <c r="F54" s="5">
+        <v>1</v>
+      </c>
       <c r="I54" t="s">
         <v>234</v>
       </c>
@@ -2018,7 +2133,9 @@
       <c r="D55" t="s">
         <v>44</v>
       </c>
-      <c r="F55" s="5"/>
+      <c r="F55" s="5">
+        <v>2</v>
+      </c>
       <c r="I55" t="s">
         <v>235</v>
       </c>
@@ -2030,7 +2147,9 @@
       <c r="D56" t="s">
         <v>45</v>
       </c>
-      <c r="F56" s="5"/>
+      <c r="F56" s="5">
+        <v>2</v>
+      </c>
       <c r="I56" t="s">
         <v>236</v>
       </c>
@@ -2042,7 +2161,9 @@
       <c r="D57" t="s">
         <v>12</v>
       </c>
-      <c r="F57" s="5"/>
+      <c r="F57" s="5">
+        <v>2</v>
+      </c>
       <c r="I57" t="s">
         <v>237</v>
       </c>
@@ -2054,7 +2175,9 @@
       <c r="C58" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F58" s="5"/>
+      <c r="F58" s="5">
+        <v>1</v>
+      </c>
       <c r="I58" t="s">
         <v>238</v>
       </c>
@@ -2066,7 +2189,9 @@
       <c r="D59" t="s">
         <v>47</v>
       </c>
-      <c r="F59" s="5"/>
+      <c r="F59" s="5">
+        <v>2</v>
+      </c>
       <c r="I59" t="s">
         <v>239</v>
       </c>
@@ -2078,7 +2203,9 @@
       <c r="D60" t="s">
         <v>44</v>
       </c>
-      <c r="F60" s="5"/>
+      <c r="F60" s="5">
+        <v>1</v>
+      </c>
       <c r="I60" t="s">
         <v>240</v>
       </c>
@@ -2090,7 +2217,9 @@
       <c r="D61" t="s">
         <v>45</v>
       </c>
-      <c r="F61" s="5"/>
+      <c r="F61" s="5">
+        <v>1</v>
+      </c>
       <c r="I61" t="s">
         <v>241</v>
       </c>
@@ -2102,7 +2231,9 @@
       <c r="D62" t="s">
         <v>12</v>
       </c>
-      <c r="F62" s="5"/>
+      <c r="F62" s="5">
+        <v>1</v>
+      </c>
       <c r="I62" t="s">
         <v>242</v>
       </c>
@@ -2114,7 +2245,9 @@
       <c r="C63" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F63" s="5"/>
+      <c r="F63" s="5">
+        <v>2</v>
+      </c>
       <c r="I63" t="s">
         <v>243</v>
       </c>
@@ -2126,7 +2259,9 @@
       <c r="D64" t="s">
         <v>47</v>
       </c>
-      <c r="F64" s="5"/>
+      <c r="F64" s="5">
+        <v>1</v>
+      </c>
       <c r="I64" t="s">
         <v>244</v>
       </c>
@@ -2138,7 +2273,9 @@
       <c r="D65" t="s">
         <v>44</v>
       </c>
-      <c r="F65" s="5"/>
+      <c r="F65" s="5">
+        <v>1</v>
+      </c>
       <c r="I65" t="s">
         <v>235</v>
       </c>
@@ -2150,7 +2287,9 @@
       <c r="D66" t="s">
         <v>50</v>
       </c>
-      <c r="F66" s="5"/>
+      <c r="F66" s="5">
+        <v>1</v>
+      </c>
       <c r="I66" t="s">
         <v>245</v>
       </c>
@@ -2162,7 +2301,9 @@
       <c r="C67" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F67" s="5"/>
+      <c r="F67" s="5">
+        <v>3</v>
+      </c>
       <c r="I67" t="s">
         <v>246</v>
       </c>
@@ -2174,7 +2315,9 @@
       <c r="D68" t="s">
         <v>47</v>
       </c>
-      <c r="F68" s="5"/>
+      <c r="F68" s="5">
+        <v>2</v>
+      </c>
       <c r="I68" t="s">
         <v>247</v>
       </c>
@@ -2186,7 +2329,9 @@
       <c r="D69" t="s">
         <v>44</v>
       </c>
-      <c r="F69" s="5"/>
+      <c r="F69" s="5">
+        <v>1</v>
+      </c>
       <c r="I69" t="s">
         <v>248</v>
       </c>
@@ -2198,7 +2343,9 @@
       <c r="D70" t="s">
         <v>45</v>
       </c>
-      <c r="F70" s="5"/>
+      <c r="F70" s="5">
+        <v>1</v>
+      </c>
       <c r="I70" t="s">
         <v>249</v>
       </c>
@@ -2210,7 +2357,9 @@
       <c r="C71" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F71" s="5"/>
+      <c r="F71" s="5">
+        <v>2</v>
+      </c>
       <c r="I71" t="s">
         <v>250</v>
       </c>
@@ -2222,7 +2371,9 @@
       <c r="D72" t="s">
         <v>47</v>
       </c>
-      <c r="F72" s="5"/>
+      <c r="F72" s="5">
+        <v>1</v>
+      </c>
       <c r="I72" t="s">
         <v>251</v>
       </c>
@@ -2234,7 +2385,9 @@
       <c r="D73" t="s">
         <v>44</v>
       </c>
-      <c r="F73" s="5"/>
+      <c r="F73" s="5">
+        <v>1</v>
+      </c>
       <c r="I73" t="s">
         <v>252</v>
       </c>
@@ -2246,7 +2399,9 @@
       <c r="D74" t="s">
         <v>45</v>
       </c>
-      <c r="F74" s="5"/>
+      <c r="F74" s="5">
+        <v>1</v>
+      </c>
       <c r="I74" t="s">
         <v>249</v>
       </c>
@@ -2267,7 +2422,9 @@
       <c r="C76" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F76" s="5"/>
+      <c r="F76" s="5">
+        <v>3</v>
+      </c>
       <c r="I76" t="s">
         <v>254</v>
       </c>
@@ -2279,7 +2436,9 @@
       <c r="D77" t="s">
         <v>47</v>
       </c>
-      <c r="F77" s="5"/>
+      <c r="F77" s="5">
+        <v>2</v>
+      </c>
       <c r="I77" t="s">
         <v>253</v>
       </c>
@@ -2291,7 +2450,9 @@
       <c r="D78" t="s">
         <v>44</v>
       </c>
-      <c r="F78" s="5"/>
+      <c r="F78" s="5">
+        <v>2</v>
+      </c>
       <c r="I78" t="s">
         <v>255</v>
       </c>
@@ -2303,7 +2464,9 @@
       <c r="C79" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F79" s="5"/>
+      <c r="F79" s="5">
+        <v>3</v>
+      </c>
       <c r="I79" t="s">
         <v>256</v>
       </c>
@@ -2315,7 +2478,9 @@
       <c r="D80" t="s">
         <v>56</v>
       </c>
-      <c r="F80" s="5"/>
+      <c r="F80" s="5">
+        <v>5</v>
+      </c>
       <c r="I80" t="s">
         <v>257</v>
       </c>
@@ -2336,7 +2501,9 @@
       <c r="C82" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F82" s="5"/>
+      <c r="F82" s="5">
+        <v>5</v>
+      </c>
       <c r="I82" t="s">
         <v>258</v>
       </c>
@@ -2348,7 +2515,9 @@
       <c r="D83" t="s">
         <v>59</v>
       </c>
-      <c r="F83" s="5"/>
+      <c r="F83" s="5">
+        <v>4</v>
+      </c>
       <c r="I83" t="s">
         <v>259</v>
       </c>
@@ -2360,7 +2529,9 @@
       <c r="D84" t="s">
         <v>60</v>
       </c>
-      <c r="F84" s="5"/>
+      <c r="F84" s="5">
+        <v>3</v>
+      </c>
       <c r="I84" t="s">
         <v>260</v>
       </c>
@@ -2372,7 +2543,9 @@
       <c r="D85" t="s">
         <v>25</v>
       </c>
-      <c r="F85" s="5"/>
+      <c r="F85" s="5">
+        <v>4</v>
+      </c>
       <c r="I85" t="s">
         <v>261</v>
       </c>
@@ -2384,7 +2557,9 @@
       <c r="C86" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F86" s="5"/>
+      <c r="F86" s="5">
+        <v>4</v>
+      </c>
       <c r="I86" t="s">
         <v>262</v>
       </c>
@@ -2396,7 +2571,9 @@
       <c r="D87" t="s">
         <v>62</v>
       </c>
-      <c r="F87" s="5"/>
+      <c r="F87" s="5">
+        <v>3</v>
+      </c>
       <c r="I87" t="s">
         <v>263</v>
       </c>
@@ -2408,7 +2585,9 @@
       <c r="D88" t="s">
         <v>60</v>
       </c>
-      <c r="F88" s="5"/>
+      <c r="F88" s="5">
+        <v>2</v>
+      </c>
       <c r="I88" t="s">
         <v>260</v>
       </c>
@@ -2420,7 +2599,9 @@
       <c r="D89" t="s">
         <v>25</v>
       </c>
-      <c r="F89" s="5"/>
+      <c r="F89" s="5">
+        <v>2</v>
+      </c>
       <c r="I89" t="s">
         <v>264</v>
       </c>
@@ -2432,7 +2613,9 @@
       <c r="C90" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F90" s="5"/>
+      <c r="F90" s="5">
+        <v>3</v>
+      </c>
       <c r="I90" t="s">
         <v>265</v>
       </c>
@@ -2444,7 +2627,9 @@
       <c r="D91" t="s">
         <v>64</v>
       </c>
-      <c r="F91" s="5"/>
+      <c r="F91" s="5">
+        <v>2</v>
+      </c>
       <c r="I91" t="s">
         <v>266</v>
       </c>
@@ -2456,7 +2641,9 @@
       <c r="D92" t="s">
         <v>65</v>
       </c>
-      <c r="F92" s="5"/>
+      <c r="F92" s="5">
+        <v>1</v>
+      </c>
       <c r="I92" t="s">
         <v>267</v>
       </c>
@@ -2468,7 +2655,9 @@
       <c r="C93" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F93" s="5"/>
+      <c r="F93" s="5">
+        <v>5</v>
+      </c>
       <c r="I93" t="s">
         <v>268</v>
       </c>
@@ -2480,7 +2669,9 @@
       <c r="D94" t="s">
         <v>66</v>
       </c>
-      <c r="F94" s="5"/>
+      <c r="F94" s="5">
+        <v>3</v>
+      </c>
       <c r="I94" t="s">
         <v>269</v>
       </c>
@@ -2492,7 +2683,9 @@
       <c r="D95" t="s">
         <v>67</v>
       </c>
-      <c r="F95" s="5"/>
+      <c r="F95" s="5">
+        <v>2</v>
+      </c>
       <c r="I95" t="s">
         <v>270</v>
       </c>
@@ -2504,7 +2697,9 @@
       <c r="D96" t="s">
         <v>35</v>
       </c>
-      <c r="F96" s="5"/>
+      <c r="F96" s="5">
+        <v>1</v>
+      </c>
       <c r="I96" t="s">
         <v>271</v>
       </c>
@@ -2517,7 +2712,9 @@
         <v>68</v>
       </c>
       <c r="D97" s="2"/>
-      <c r="F97" s="5"/>
+      <c r="F97" s="5">
+        <v>16</v>
+      </c>
       <c r="I97" t="s">
         <v>272</v>
       </c>
@@ -2539,7 +2736,9 @@
         <v>70</v>
       </c>
       <c r="D99" s="2"/>
-      <c r="F99" s="5"/>
+      <c r="F99" s="5">
+        <v>4</v>
+      </c>
       <c r="I99" t="s">
         <v>273</v>
       </c>
@@ -2551,7 +2750,9 @@
       <c r="D100" t="s">
         <v>71</v>
       </c>
-      <c r="F100" s="5"/>
+      <c r="F100" s="5">
+        <v>8</v>
+      </c>
       <c r="I100" t="s">
         <v>274</v>
       </c>
@@ -2564,7 +2765,9 @@
         <v>72</v>
       </c>
       <c r="D101" s="4"/>
-      <c r="F101" s="5"/>
+      <c r="F101" s="5">
+        <v>3</v>
+      </c>
       <c r="I101" t="s">
         <v>275</v>
       </c>
@@ -2576,7 +2779,9 @@
       <c r="D102" t="s">
         <v>73</v>
       </c>
-      <c r="F102" s="5"/>
+      <c r="F102" s="5">
+        <v>3</v>
+      </c>
       <c r="I102" t="s">
         <v>276</v>
       </c>
@@ -2588,7 +2793,9 @@
       <c r="D103" t="s">
         <v>74</v>
       </c>
-      <c r="F103" s="5"/>
+      <c r="F103" s="5">
+        <v>2</v>
+      </c>
       <c r="I103" t="s">
         <v>277</v>
       </c>
@@ -2600,7 +2807,9 @@
       <c r="C104" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F104" s="5"/>
+      <c r="F104" s="5">
+        <v>6</v>
+      </c>
       <c r="I104" t="s">
         <v>278</v>
       </c>
@@ -2612,7 +2821,9 @@
       <c r="D105" t="s">
         <v>76</v>
       </c>
-      <c r="F105" s="5"/>
+      <c r="F105" s="5">
+        <v>3</v>
+      </c>
       <c r="I105" t="s">
         <v>279</v>
       </c>
@@ -2624,7 +2835,9 @@
       <c r="D106" t="s">
         <v>77</v>
       </c>
-      <c r="F106" s="5"/>
+      <c r="F106" s="5">
+        <v>3</v>
+      </c>
       <c r="I106" t="s">
         <v>280</v>
       </c>
@@ -2636,7 +2849,9 @@
       <c r="C107" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F107" s="5"/>
+      <c r="F107" s="5">
+        <v>8</v>
+      </c>
       <c r="I107" t="s">
         <v>281</v>
       </c>
@@ -2648,7 +2863,9 @@
       <c r="D108" t="s">
         <v>27</v>
       </c>
-      <c r="F108" s="5"/>
+      <c r="F108" s="5">
+        <v>4</v>
+      </c>
       <c r="I108" t="s">
         <v>282</v>
       </c>
@@ -2660,7 +2877,9 @@
       <c r="D109" t="s">
         <v>79</v>
       </c>
-      <c r="F109" s="5"/>
+      <c r="F109" s="5">
+        <v>3</v>
+      </c>
       <c r="I109" t="s">
         <v>283</v>
       </c>
@@ -2672,7 +2891,9 @@
       <c r="D110" t="s">
         <v>60</v>
       </c>
-      <c r="F110" s="5"/>
+      <c r="F110" s="5">
+        <v>3</v>
+      </c>
       <c r="I110" t="s">
         <v>284</v>
       </c>
@@ -2684,7 +2905,9 @@
       <c r="D111" t="s">
         <v>80</v>
       </c>
-      <c r="F111" s="5"/>
+      <c r="F111" s="5">
+        <v>3</v>
+      </c>
       <c r="I111" t="s">
         <v>285</v>
       </c>
@@ -2696,7 +2919,9 @@
       <c r="D112" t="s">
         <v>26</v>
       </c>
-      <c r="F112" s="5"/>
+      <c r="F112" s="5">
+        <v>3</v>
+      </c>
       <c r="I112" t="s">
         <v>286</v>
       </c>
@@ -2708,7 +2933,9 @@
       <c r="D113" t="s">
         <v>81</v>
       </c>
-      <c r="F113" s="5"/>
+      <c r="F113" s="5">
+        <v>3</v>
+      </c>
       <c r="I113" t="s">
         <v>287</v>
       </c>
@@ -2729,7 +2956,9 @@
       <c r="C115" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F115" s="5"/>
+      <c r="F115" s="5">
+        <v>16</v>
+      </c>
       <c r="I115" t="s">
         <v>288</v>
       </c>
@@ -2741,7 +2970,9 @@
       <c r="D116" t="s">
         <v>57</v>
       </c>
-      <c r="F116" s="5"/>
+      <c r="F116" s="5">
+        <v>8</v>
+      </c>
       <c r="I116" t="s">
         <v>289</v>
       </c>
@@ -2753,7 +2984,9 @@
       <c r="D117" t="s">
         <v>84</v>
       </c>
-      <c r="F117" s="5"/>
+      <c r="F117" s="5">
+        <v>3</v>
+      </c>
       <c r="I117" t="s">
         <v>290</v>
       </c>
@@ -2765,7 +2998,9 @@
       <c r="D118" t="s">
         <v>85</v>
       </c>
-      <c r="F118" s="5"/>
+      <c r="F118" s="5">
+        <v>3</v>
+      </c>
       <c r="I118" t="s">
         <v>291</v>
       </c>
@@ -2777,7 +3012,9 @@
       <c r="D119" t="s">
         <v>86</v>
       </c>
-      <c r="F119" s="5"/>
+      <c r="F119" s="5">
+        <v>1</v>
+      </c>
       <c r="I119" t="s">
         <v>292</v>
       </c>
@@ -2789,7 +3026,9 @@
       <c r="D120" t="s">
         <v>87</v>
       </c>
-      <c r="F120" s="5"/>
+      <c r="F120" s="5">
+        <v>1</v>
+      </c>
       <c r="I120" t="s">
         <v>293</v>
       </c>
@@ -2801,7 +3040,9 @@
       <c r="C121" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F121" s="5"/>
+      <c r="F121" s="5">
+        <v>8</v>
+      </c>
       <c r="I121" t="s">
         <v>294</v>
       </c>
@@ -2813,7 +3054,9 @@
       <c r="D122" t="s">
         <v>89</v>
       </c>
-      <c r="F122" s="5"/>
+      <c r="F122" s="5">
+        <v>3</v>
+      </c>
       <c r="I122" t="s">
         <v>295</v>
       </c>
@@ -2825,7 +3068,9 @@
       <c r="D123" t="s">
         <v>90</v>
       </c>
-      <c r="F123" s="5"/>
+      <c r="F123" s="5">
+        <v>1</v>
+      </c>
       <c r="I123" t="s">
         <v>296</v>
       </c>
@@ -2837,7 +3082,9 @@
       <c r="D124" t="s">
         <v>91</v>
       </c>
-      <c r="F124" s="5"/>
+      <c r="F124" s="5">
+        <v>1</v>
+      </c>
       <c r="I124" t="s">
         <v>297</v>
       </c>
@@ -2859,7 +3106,9 @@
         <v>93</v>
       </c>
       <c r="D126" s="2"/>
-      <c r="F126" s="5"/>
+      <c r="F126" s="5">
+        <v>1</v>
+      </c>
       <c r="I126" t="s">
         <v>298</v>
       </c>
@@ -2871,7 +3120,9 @@
       <c r="D127" t="s">
         <v>94</v>
       </c>
-      <c r="F127" s="5"/>
+      <c r="F127" s="5">
+        <v>1</v>
+      </c>
       <c r="I127" t="s">
         <v>299</v>
       </c>
@@ -2883,7 +3134,9 @@
       <c r="D128" t="s">
         <v>95</v>
       </c>
-      <c r="F128" s="5"/>
+      <c r="F128" s="5">
+        <v>1</v>
+      </c>
       <c r="I128" t="s">
         <v>300</v>
       </c>
@@ -2895,7 +3148,9 @@
       <c r="C129" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F129" s="5"/>
+      <c r="F129" s="5">
+        <v>2</v>
+      </c>
       <c r="I129" t="s">
         <v>301</v>
       </c>
@@ -2907,7 +3162,9 @@
       <c r="D130" t="s">
         <v>96</v>
       </c>
-      <c r="F130" s="5"/>
+      <c r="F130" s="5">
+        <v>1</v>
+      </c>
       <c r="I130" t="s">
         <v>302</v>
       </c>
@@ -2919,7 +3176,9 @@
       <c r="D131" t="s">
         <v>97</v>
       </c>
-      <c r="F131" s="5"/>
+      <c r="F131" s="5">
+        <v>1</v>
+      </c>
       <c r="I131" t="s">
         <v>303</v>
       </c>
@@ -2932,9 +3191,20 @@
         <v>98</v>
       </c>
       <c r="D132" s="2"/>
-      <c r="F132" s="5"/>
+      <c r="F132" s="5">
+        <v>2</v>
+      </c>
       <c r="I132" t="s">
         <v>304</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C133" t="s">
+        <v>305</v>
+      </c>
+      <c r="F133" s="7">
+        <f>SUM(F4:F132)</f>
+        <v>301</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ytterligare uppdatering av WBS
</commit_message>
<xml_diff>
--- a/Bolaget/Temp/WBS v.1.xlsx
+++ b/Bolaget/Temp/WBS v.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beije\Documents\Projektkurs DVA227\Bolaget\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAD704B-BE94-445C-91D4-6F20D7D4CF89}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB1B19D4-B587-4DA5-8687-F8A6826B0E88}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5784" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="331">
   <si>
     <t>Nätverkstjänster</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Protokoll</t>
   </si>
   <si>
-    <t>Dot.1x</t>
-  </si>
-  <si>
     <t>Kryptering</t>
   </si>
   <si>
@@ -237,15 +234,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>Rätt access</t>
-  </si>
-  <si>
-    <t>Konnektivitet</t>
-  </si>
-  <si>
-    <t>MGMT</t>
-  </si>
-  <si>
     <t>Mässa</t>
   </si>
   <si>
@@ -354,9 +342,6 @@
     <t>Utbilda personalen som arbetar på plats, ska det vara en konsult som åker ut eller en lokal förmåga?</t>
   </si>
   <si>
-    <t>Definiera admin access</t>
-  </si>
-  <si>
     <t>Vilka personer räknas som admin, ska det finnas en lokal admin på varje site?</t>
   </si>
   <si>
@@ -735,9 +720,6 @@
     <t>Vad är nuvarande best-practive när det kommer till mjukvara?</t>
   </si>
   <si>
-    <t>Design av routingtabeller och hur nätverket ska se ut</t>
-  </si>
-  <si>
     <t>Sätta upp IP-plan, både site-specifikt och generellt för intranät och VPN</t>
   </si>
   <si>
@@ -756,18 +738,12 @@
     <t>Vilka switchingprotokoll ska användas? Går också att sammankoppla med säkerhet.</t>
   </si>
   <si>
-    <t>Trådlöst näst, design av accesstillgång till trådlöst nät</t>
-  </si>
-  <si>
     <t>Standardisera placering och mängd av accesspunkter?</t>
   </si>
   <si>
     <t>Hur löser man wireless-ap tillsammans med PoE?</t>
   </si>
   <si>
-    <t>Generell redundans punkt, hur mycket redundans krävs generellt över nätverket både inom nätverk och nätverkstjänster</t>
-  </si>
-  <si>
     <t>Hur mycket redundans är möjlig?</t>
   </si>
   <si>
@@ -780,33 +756,21 @@
     <t>Standardisering av designen för enkelt roll-out på andra siter.</t>
   </si>
   <si>
-    <t>Vem sköter installationen</t>
-  </si>
-  <si>
     <t>Hur går installationen till?</t>
   </si>
   <si>
-    <t>Hur löser vi frakt och logistik till hela världen?</t>
-  </si>
-  <si>
     <t>Risker med frakt, hur tar man hänsyn till dom?</t>
   </si>
   <si>
     <t>Tid för frakt och logistik</t>
   </si>
   <si>
-    <t>Stegplan för implementationen</t>
-  </si>
-  <si>
     <t>I vilken ordning utför man arbetet?</t>
   </si>
   <si>
     <t>Den måste vara välskriven och inituitiv, hur löser vi det?</t>
   </si>
   <si>
-    <t>Hur man går tillväga för att undersöka så att nätverket fungerar som det ska</t>
-  </si>
-  <si>
     <t>Hur man testar krypteringen</t>
   </si>
   <si>
@@ -825,9 +789,6 @@
     <t>Hur man testar så att MGMT-nätet bara innehåller MGMT-trafik</t>
   </si>
   <si>
-    <t>På mässan behöver vi en monter</t>
-  </si>
-  <si>
     <t>Designa monter som visar vad vi har gjort och kommit fram till</t>
   </si>
   <si>
@@ -843,9 +804,6 @@
     <t>Frakt från utställningen till soptunna</t>
   </si>
   <si>
-    <t>En utställning kan få bättre respons om det finns merchendise tillgängligt</t>
-  </si>
-  <si>
     <t>Designa flyers med sammanfattningar av arbetet</t>
   </si>
   <si>
@@ -855,18 +813,12 @@
     <t>Köpa godis?</t>
   </si>
   <si>
-    <t>Skriva dagbok och dokumentera arbetsuppgifter</t>
-  </si>
-  <si>
     <t>Ha ett gruppmöte I veckan med konstant dokumentation av diskuterade punkter och beslut</t>
   </si>
   <si>
     <t>Dagböcker där arbetsuppgifter och utfört arbete skrivs ner för att dokumenteras</t>
   </si>
   <si>
-    <t>Planering av skrivningen av rapporten, när ska vi börja osv</t>
-  </si>
-  <si>
     <t>Startdatum för rapporten</t>
   </si>
   <si>
@@ -891,9 +843,6 @@
     <t>Varaktighet (dagar)</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>2.1.2</t>
   </si>
   <si>
@@ -1021,6 +970,54 @@
   </si>
   <si>
     <t>IP-plan för routing</t>
+  </si>
+  <si>
+    <t>Vem ska installera</t>
+  </si>
+  <si>
+    <t>Vem sköter installationen, lokal förmåga eller konsult som åker ut och fixar</t>
+  </si>
+  <si>
+    <t>Bolad</t>
+  </si>
+  <si>
+    <t>Vem kan skicka till hela världen? Behövs olika bolag?</t>
+  </si>
+  <si>
+    <t>Krypteringstest</t>
+  </si>
+  <si>
+    <t>Rätt access-test</t>
+  </si>
+  <si>
+    <t>Redundanstest</t>
+  </si>
+  <si>
+    <t>Konnektivitetstest</t>
+  </si>
+  <si>
+    <t>Dot.1x-test</t>
+  </si>
+  <si>
+    <t>MGMT-test</t>
+  </si>
+  <si>
+    <t>6.1.5</t>
+  </si>
+  <si>
+    <t>VLAN</t>
+  </si>
+  <si>
+    <t>Vilka olika VLAN ska finnas på nätet. Avgränsningar osv.</t>
+  </si>
+  <si>
+    <t>7.2.3</t>
+  </si>
+  <si>
+    <t>VLAN-test</t>
+  </si>
+  <si>
+    <t>Hur testar man så att alla VLAN gör det dom ska?</t>
   </si>
 </sst>
 </file>
@@ -1421,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I140"/>
+  <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D89" sqref="D89"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I143" sqref="I143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1434,26 +1431,27 @@
     <col min="5" max="5" width="109.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="G1" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="H1" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="I1" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1473,7 +1471,7 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I4">
         <v>4</v>
@@ -1487,21 +1485,18 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5">
-        <v>4</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -1509,13 +1504,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -1523,13 +1518,13 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -1537,13 +1532,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1551,13 +1546,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1565,13 +1560,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -1579,13 +1574,13 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -1593,13 +1588,13 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I13">
         <v>1</v>
@@ -1607,13 +1602,13 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1634,19 +1629,16 @@
       <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D17" t="s">
         <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I17">
         <v>1</v>
@@ -1654,13 +1646,16 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>289</v>
+        <v>272</v>
       </c>
       <c r="D18" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
       <c r="E18" t="s">
-        <v>291</v>
+        <v>274</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1671,19 +1666,16 @@
         <v>15</v>
       </c>
       <c r="D19" s="2"/>
-      <c r="I19">
-        <v>1</v>
-      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -1691,13 +1683,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D21" t="s">
         <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -1711,19 +1703,16 @@
         <v>18</v>
       </c>
       <c r="D22" s="3"/>
-      <c r="I22">
-        <v>1</v>
-      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E23" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I23">
         <v>1</v>
@@ -1731,13 +1720,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I24">
         <v>1</v>
@@ -1745,24 +1734,27 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E25" t="s">
-        <v>105</v>
+        <v>101</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E26" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I26">
         <v>1</v>
@@ -1776,22 +1768,16 @@
         <v>22</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" t="s">
-        <v>109</v>
-      </c>
-      <c r="I27">
-        <v>2</v>
-      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D28" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="E28" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="I28">
         <v>1</v>
@@ -1799,13 +1785,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D29" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="E29" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="I29">
         <v>1</v>
@@ -1813,13 +1799,13 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D30" t="s">
-        <v>294</v>
+        <v>277</v>
       </c>
       <c r="E30" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="I30">
         <v>1</v>
@@ -1832,19 +1818,16 @@
       <c r="C31" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I31">
-        <v>4</v>
-      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D32" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="E32" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="I32">
         <v>2</v>
@@ -1852,13 +1835,13 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D33" t="s">
-        <v>296</v>
+        <v>279</v>
       </c>
       <c r="E33" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I33">
         <v>2</v>
@@ -1866,13 +1849,13 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="I34">
         <v>2</v>
@@ -1883,21 +1866,18 @@
         <v>2.6</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I35">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E36" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="I36">
         <v>1</v>
@@ -1905,13 +1885,16 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="D37" t="s">
-        <v>298</v>
+        <v>281</v>
       </c>
       <c r="E37" t="s">
-        <v>116</v>
+        <v>111</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1919,7 +1902,7 @@
         <v>3</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -1927,21 +1910,18 @@
         <v>3.1</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I39">
-        <v>1</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E40" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I40">
         <v>1</v>
@@ -1949,16 +1929,16 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E41" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="I41">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -1966,21 +1946,18 @@
         <v>3.2</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I42">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D43" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E43" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="I43">
         <v>1</v>
@@ -1988,13 +1965,13 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E44" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I44">
         <v>3</v>
@@ -2005,7 +1982,7 @@
         <v>3.3</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I45">
         <v>3</v>
@@ -2013,27 +1990,24 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D46" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="E46" t="s">
-        <v>122</v>
-      </c>
-      <c r="I46">
-        <v>3</v>
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D47" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="E47" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="I47">
         <v>2</v>
@@ -2044,22 +2018,19 @@
         <v>3.4</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D48" s="4"/>
-      <c r="I48">
-        <v>2</v>
-      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D49" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="E49" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I49">
         <v>2</v>
@@ -2067,24 +2038,30 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="D50" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="E50" t="s">
-        <v>306</v>
+        <v>289</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="D51" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="E51" t="s">
-        <v>305</v>
+        <v>288</v>
+      </c>
+      <c r="I51">
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -2092,7 +2069,7 @@
         <v>4</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -2100,22 +2077,19 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D53" s="2"/>
-      <c r="I53">
-        <v>3</v>
-      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D54" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="E54" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="I54">
         <v>2</v>
@@ -2123,13 +2097,13 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D55" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="E55" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="I55">
         <v>2</v>
@@ -2137,13 +2111,13 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D56" t="s">
-        <v>310</v>
+        <v>293</v>
       </c>
       <c r="E56" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="I56">
         <v>1</v>
@@ -2151,13 +2125,13 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D57" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
       <c r="E57" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="I57">
         <v>2</v>
@@ -2168,21 +2142,18 @@
         <v>4.2</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I58">
-        <v>1</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D59" t="s">
-        <v>312</v>
+        <v>295</v>
       </c>
       <c r="E59" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="I59">
         <v>1</v>
@@ -2190,13 +2161,13 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D60" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="E60" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="I60">
         <v>2</v>
@@ -2204,13 +2175,13 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D61" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
       <c r="E61" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="I61">
         <v>2</v>
@@ -2218,13 +2189,13 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D62" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="E62" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I62">
         <v>2</v>
@@ -2235,21 +2206,18 @@
         <v>4.3</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I63">
-        <v>1</v>
+        <v>41</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D64" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
       <c r="E64" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="I64">
         <v>2</v>
@@ -2257,13 +2225,13 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="D65" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="E65" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I65">
         <v>1</v>
@@ -2271,13 +2239,13 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D66" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="E66" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I66">
         <v>1</v>
@@ -2285,13 +2253,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D67" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="E67" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="I67">
         <v>1</v>
@@ -2302,21 +2270,18 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I68">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D69" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="E69" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I69">
         <v>1</v>
@@ -2324,13 +2289,13 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D70" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="E70" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="I70">
         <v>1</v>
@@ -2338,13 +2303,13 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D71" t="s">
-        <v>322</v>
+        <v>305</v>
       </c>
       <c r="E71" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="I71">
         <v>1</v>
@@ -2355,21 +2320,18 @@
         <v>4.5</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I72">
-        <v>3</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D73" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E73" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="I73">
         <v>2</v>
@@ -2377,13 +2339,13 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D74" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E74" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="I74">
         <v>1</v>
@@ -2391,13 +2353,13 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="D75" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E75" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="I75">
         <v>1</v>
@@ -2408,21 +2370,18 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I76">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D77" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E77" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="I77">
         <v>1</v>
@@ -2430,13 +2389,13 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D78" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E78" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="I78">
         <v>1</v>
@@ -2444,13 +2403,13 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D79" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E79" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="I79">
         <v>1</v>
@@ -2461,7 +2420,7 @@
         <v>5</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -2469,24 +2428,21 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E81" t="s">
-        <v>232</v>
-      </c>
-      <c r="I81">
-        <v>3</v>
+        <v>227</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D82" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="E82" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="I82">
         <v>2</v>
@@ -2494,13 +2450,13 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D83" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="E83" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="I83">
         <v>2</v>
@@ -2511,24 +2467,21 @@
         <v>5.2</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E84" t="s">
-        <v>234</v>
-      </c>
-      <c r="I84">
-        <v>3</v>
+        <v>229</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="5" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D85" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="E85" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="I85">
         <v>5</v>
@@ -2539,7 +2492,7 @@
         <v>6</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
@@ -2547,27 +2500,18 @@
         <v>6.1</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E87" t="s">
-        <v>236</v>
-      </c>
-      <c r="H87" t="s">
-        <v>288</v>
-      </c>
-      <c r="I87">
-        <v>5</v>
+        <v>49</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D88" t="s">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="E88" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="I88">
         <v>4</v>
@@ -2575,13 +2519,13 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D89" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E89" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="I89">
         <v>3</v>
@@ -2589,13 +2533,13 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D90" t="s">
         <v>23</v>
       </c>
       <c r="E90" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="I90">
         <v>4</v>
@@ -2603,66 +2547,63 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D91" t="s">
+        <v>310</v>
+      </c>
+      <c r="E91" t="s">
+        <v>311</v>
+      </c>
+      <c r="I91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="D92" t="s">
         <v>326</v>
       </c>
-      <c r="D91" t="s">
+      <c r="E92" t="s">
         <v>327</v>
       </c>
-      <c r="E91" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="5">
+      <c r="I92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A93" s="5">
         <v>6.2</v>
       </c>
-      <c r="C92" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E92" t="s">
-        <v>240</v>
-      </c>
-      <c r="I92">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="D93" t="s">
-        <v>53</v>
-      </c>
-      <c r="E93" t="s">
-        <v>241</v>
-      </c>
-      <c r="I93">
-        <v>3</v>
+      <c r="C93" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="5" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D94" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E94" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="I94">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="5" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D95" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="E95" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="I95">
         <v>2</v>
@@ -2670,474 +2611,432 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="5" t="s">
-        <v>329</v>
+        <v>182</v>
       </c>
       <c r="D96" t="s">
-        <v>330</v>
+        <v>23</v>
+      </c>
+      <c r="E96" t="s">
+        <v>236</v>
+      </c>
+      <c r="I96">
+        <v>2</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="5">
-        <v>6.3</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>54</v>
+      <c r="A97" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="D97" t="s">
+        <v>313</v>
       </c>
       <c r="E97" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="I97">
         <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="D98" t="s">
-        <v>55</v>
-      </c>
-      <c r="E98" t="s">
-        <v>244</v>
-      </c>
-      <c r="I98">
-        <v>2</v>
+      <c r="A98" s="5">
+        <v>6.3</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D99" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E99" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="I99">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="5">
+      <c r="A100" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="D100" t="s">
+        <v>55</v>
+      </c>
+      <c r="E100" t="s">
+        <v>238</v>
+      </c>
+      <c r="I100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A101" s="5">
         <v>6.4</v>
       </c>
-      <c r="C100" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E100" t="s">
-        <v>246</v>
-      </c>
-      <c r="I100">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="D101" t="s">
-        <v>57</v>
-      </c>
-      <c r="E101" t="s">
-        <v>247</v>
-      </c>
-      <c r="I101">
-        <v>3</v>
+      <c r="C101" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D102" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E102" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="I102">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D103" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="E103" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="I103">
         <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="5">
-        <v>6.5</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D104" s="2"/>
+      <c r="A104" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D104" t="s">
+        <v>32</v>
+      </c>
       <c r="E104" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="I104">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="5">
-        <v>7</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>60</v>
+        <v>6.5</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D105" s="2"/>
+      <c r="E105" t="s">
+        <v>242</v>
+      </c>
+      <c r="I105">
+        <v>16</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="5">
+        <v>7</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A107" s="5">
         <v>7.1</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C107" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D107" s="2"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A108" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D108" t="s">
         <v>61</v>
       </c>
-      <c r="D106" s="2"/>
-      <c r="E106" t="s">
-        <v>251</v>
-      </c>
-      <c r="I106">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="D107" t="s">
+      <c r="E108" t="s">
+        <v>243</v>
+      </c>
+      <c r="I108">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D109" t="s">
+        <v>315</v>
+      </c>
+      <c r="E109" t="s">
+        <v>316</v>
+      </c>
+      <c r="I109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A110" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="C110" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E107" t="s">
-        <v>252</v>
-      </c>
-      <c r="I107">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="5">
-        <v>7.2</v>
-      </c>
-      <c r="C108" s="4" t="s">
+      <c r="D110" s="4"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A111" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D111" t="s">
         <v>63</v>
       </c>
-      <c r="D108" s="4"/>
-      <c r="E108" t="s">
-        <v>253</v>
-      </c>
-      <c r="I108">
+      <c r="E111" t="s">
+        <v>244</v>
+      </c>
+      <c r="I111">
         <v>3</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="D109" t="s">
-        <v>64</v>
-      </c>
-      <c r="E109" t="s">
-        <v>254</v>
-      </c>
-      <c r="I109">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D110" t="s">
-        <v>65</v>
-      </c>
-      <c r="E110" t="s">
-        <v>255</v>
-      </c>
-      <c r="I110">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="5">
-        <v>7.3</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E111" t="s">
-        <v>256</v>
-      </c>
-      <c r="I111">
-        <v>6</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D112" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E112" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="I112">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="s">
-        <v>197</v>
+        <v>328</v>
       </c>
       <c r="D113" t="s">
-        <v>68</v>
+        <v>317</v>
       </c>
       <c r="E113" t="s">
-        <v>258</v>
+        <v>318</v>
       </c>
       <c r="I113">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="5">
-        <v>7.4</v>
-      </c>
-      <c r="C114" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E114" t="s">
-        <v>259</v>
-      </c>
-      <c r="I114">
-        <v>8</v>
+        <v>7.3</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="5" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D115" t="s">
-        <v>25</v>
+        <v>66</v>
       </c>
       <c r="E115" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="I115">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="5" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="D116" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E116" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="I116">
         <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="D117" t="s">
-        <v>51</v>
-      </c>
-      <c r="E117" t="s">
-        <v>262</v>
-      </c>
-      <c r="I117">
-        <v>3</v>
+      <c r="A117" s="5">
+        <v>7.4</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="5" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="D118" t="s">
-        <v>71</v>
+        <v>319</v>
       </c>
       <c r="E118" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="I118">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="5" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D119" t="s">
-        <v>24</v>
+        <v>320</v>
       </c>
       <c r="E119" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="I119">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="5" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D120" t="s">
-        <v>72</v>
+        <v>321</v>
       </c>
       <c r="E120" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="I120">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="5">
-        <v>8</v>
-      </c>
-      <c r="B121" s="1" t="s">
-        <v>73</v>
+      <c r="A121" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D121" t="s">
+        <v>322</v>
+      </c>
+      <c r="E121" t="s">
+        <v>251</v>
+      </c>
+      <c r="I121">
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="5">
-        <v>8.1</v>
-      </c>
-      <c r="C122" s="2" t="s">
-        <v>74</v>
+      <c r="A122" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D122" t="s">
+        <v>323</v>
       </c>
       <c r="E122" t="s">
-        <v>266</v>
+        <v>252</v>
       </c>
       <c r="I122">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="5" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D123" t="s">
-        <v>49</v>
+        <v>324</v>
       </c>
       <c r="E123" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="I123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D124" t="s">
+        <v>329</v>
+      </c>
+      <c r="E124" t="s">
+        <v>330</v>
+      </c>
+      <c r="I124">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A125" s="5">
         <v>8</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="D124" t="s">
-        <v>75</v>
-      </c>
-      <c r="E124" t="s">
-        <v>268</v>
-      </c>
-      <c r="I124">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A125" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D125" t="s">
-        <v>76</v>
-      </c>
-      <c r="E125" t="s">
-        <v>269</v>
-      </c>
-      <c r="I125">
-        <v>3</v>
+      <c r="B125" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A126" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="D126" t="s">
-        <v>77</v>
-      </c>
-      <c r="E126" t="s">
-        <v>270</v>
-      </c>
-      <c r="I126">
-        <v>1</v>
+      <c r="A126" s="5">
+        <v>8.1</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="5" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="D127" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="E127" t="s">
-        <v>271</v>
+        <v>254</v>
       </c>
       <c r="I127">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A128" s="5">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="C128" s="3" t="s">
-        <v>79</v>
+      <c r="A128" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D128" t="s">
+        <v>71</v>
       </c>
       <c r="E128" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="I128">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="5" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D129" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E129" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="I129">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="5" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D130" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E130" t="s">
-        <v>274</v>
+        <v>257</v>
       </c>
       <c r="I130">
         <v>1</v>
@@ -3145,13 +3044,13 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="5" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="D131" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E131" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="I131">
         <v>1</v>
@@ -3159,36 +3058,35 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="5">
-        <v>9</v>
-      </c>
-      <c r="B132" s="1" t="s">
-        <v>83</v>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A133" s="5">
-        <v>9.1</v>
-      </c>
-      <c r="C133" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D133" s="2"/>
+      <c r="A133" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D133" t="s">
+        <v>76</v>
+      </c>
       <c r="E133" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="I133">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="D134" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E134" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="I134">
         <v>1</v>
@@ -3196,13 +3094,13 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D135" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E135" t="s">
-        <v>278</v>
+        <v>261</v>
       </c>
       <c r="I135">
         <v>1</v>
@@ -3210,68 +3108,107 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="5">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E136" t="s">
-        <v>279</v>
-      </c>
-      <c r="I136">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A137" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="D137" t="s">
-        <v>87</v>
-      </c>
-      <c r="E137" t="s">
-        <v>280</v>
-      </c>
-      <c r="I137">
-        <v>1</v>
-      </c>
+      <c r="A137" s="5">
+        <v>9.1</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D137" s="2"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="5" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D138" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E138" t="s">
-        <v>281</v>
+        <v>262</v>
       </c>
       <c r="I138">
         <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A139" s="5">
+      <c r="A139" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D139" t="s">
+        <v>82</v>
+      </c>
+      <c r="E139" t="s">
+        <v>263</v>
+      </c>
+      <c r="I139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A140" s="5">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A141" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D141" t="s">
+        <v>83</v>
+      </c>
+      <c r="E141" t="s">
+        <v>264</v>
+      </c>
+      <c r="I141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A142" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D142" t="s">
+        <v>84</v>
+      </c>
+      <c r="E142" t="s">
+        <v>265</v>
+      </c>
+      <c r="I142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A143" s="5">
         <v>9.3000000000000007</v>
       </c>
-      <c r="C139" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D139" s="2"/>
-      <c r="E139" t="s">
-        <v>282</v>
-      </c>
-      <c r="I139">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C140" t="s">
-        <v>283</v>
-      </c>
-      <c r="I140">
-        <f>SUM(I4:I139)</f>
-        <v>301</v>
+      <c r="C143" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D143" s="2"/>
+      <c r="E143" t="s">
+        <v>266</v>
+      </c>
+      <c r="I143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C144" t="s">
+        <v>267</v>
+      </c>
+      <c r="I144">
+        <f>SUM(I4:I143)</f>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>